<commit_message>
added ureponly UI and hooks
</commit_message>
<xml_diff>
--- a/fixtures/input/urec.xlsx
+++ b/fixtures/input/urec.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaker\Documents\HEM4Python\Version1.0\sample files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3C89A-DB78-4DD4-873F-E217F0917387}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" xr2:uid="{D576B197-8000-406B-9A1B-60EA6691BF52}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="7668" xr2:uid="{D576B197-8000-406B-9A1B-60EA6691BF52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Facility ID</t>
   </si>
@@ -60,6 +62,12 @@
   </si>
   <si>
     <t>RECPTID2</t>
+  </si>
+  <si>
+    <t>Hill height</t>
+  </si>
+  <si>
+    <t>Population</t>
   </si>
 </sst>
 </file>
@@ -97,12 +105,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -112,6 +114,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -164,10 +174,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,12 +497,12 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,12 +527,16 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -549,5 +564,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>